<commit_message>
large modification, config4.json intro. Research about softAP mode.
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDEBA3C-4D63-4058-86CA-F076FD57356F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5B99E0-C313-43B5-9179-E45E2D681B48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="2430" windowWidth="13365" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comon tests" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
   <si>
     <t>Nom du test</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Mode manual RED ON/OFF simple via HTML</t>
-  </si>
-  <si>
-    <t>Mode manual RED ON/OFF simple vie BP</t>
   </si>
   <si>
     <t>Attenus</t>
@@ -263,12 +260,48 @@
   <si>
     <t>Test under tablette and PC and phone</t>
   </si>
+  <si>
+    <t>ac02290</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Mode manual RED ON/OFF simple via BP</t>
+  </si>
+  <si>
+    <t>Ne pas remplir le champ</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>Pas de prise en compte</t>
+  </si>
+  <si>
+    <t>Ne pas être transmis</t>
+  </si>
+  <si>
+    <t>Cleanup button</t>
+  </si>
+  <si>
+    <t>Arret checked and all others field removed</t>
+  </si>
+  <si>
+    <t>WiFi Ok mais pas d'internet</t>
+  </si>
+  <si>
+    <t>Pas de json pour l'interface</t>
+  </si>
+  <si>
+    <t>passer à la version light de l'interface</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,13 +317,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -302,10 +355,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -313,8 +368,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -328,6 +394,164 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F9365E-C82A-4A20-B8BD-7E202C3B0026}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9525000" y="762000"/>
+          <a:ext cx="4781550" cy="2990850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Erreur gérées par la classe CSystemStatus et l'instance systemStatus.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>attributs:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errWifi</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errInternet</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errNtp</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errI2C</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errRTC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>errNano</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>err</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>SPIFFS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>errConfigFile</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Méthodes public</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>allIsOk()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Peut-être getGravityError()</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -595,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6009E7-5EB8-4E17-B18A-0866A3019060}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -612,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -626,40 +850,40 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -669,10 +893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A8B8F9-5134-4744-A58F-404FFAC0FBF4}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +904,7 @@
     <col min="1" max="1" width="60.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
     <col min="5" max="6" width="11.42578125" style="1"/>
     <col min="7" max="7" width="17.7109375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
@@ -691,13 +915,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -714,146 +938,246 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>76</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>79</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="3">
+        <v>43558</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -864,171 +1188,189 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="B17" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CSysStatus class introduction + power up debug !!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!!
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5B99E0-C313-43B5-9179-E45E2D681B48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF8C8BC-A0E1-44F6-BB2A-29EEC004EE1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comon tests" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
   <si>
     <t>Nom du test</t>
   </si>
@@ -159,9 +159,6 @@
     <t>RTC tests</t>
   </si>
   <si>
-    <t>First boot test</t>
-  </si>
-  <si>
     <t>All LED off</t>
   </si>
   <si>
@@ -295,6 +292,27 @@
   </si>
   <si>
     <t>passer à la version light de l'interface</t>
+  </si>
+  <si>
+    <t>First boot tests: normal, SSID connect</t>
+  </si>
+  <si>
+    <t>First boot tests: normal, SSID connect wrong cred</t>
+  </si>
+  <si>
+    <t>First boot tests: normal, AP mode</t>
+  </si>
+  <si>
+    <t>First boot tests: normal, AP mode too short pass</t>
+  </si>
+  <si>
+    <t>First boot tests: normal, AP mode too long pass</t>
+  </si>
+  <si>
+    <t>I2C recovery</t>
+  </si>
+  <si>
+    <t>I2C recovery : 3 error max =&gt; fatal error</t>
   </si>
 </sst>
 </file>
@@ -817,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6009E7-5EB8-4E17-B18A-0866A3019060}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +881,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -878,12 +896,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A8B8F9-5134-4744-A58F-404FFAC0FBF4}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -944,18 +992,18 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="3">
         <v>43558</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -964,13 +1012,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3">
         <v>43558</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -984,13 +1032,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F4" s="3">
         <v>43558</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -998,19 +1046,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="F5" s="3">
         <v>43558</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1021,19 +1069,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="3">
         <v>43558</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1044,13 +1092,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="3">
         <v>43558</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1061,33 +1109,33 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F8" s="3">
         <v>43558</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F9" s="3">
         <v>43558</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1098,7 +1146,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1190,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1203,167 +1251,167 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
         <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
         <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
         <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
         <v>80</v>
       </c>
-      <c r="B18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>81</v>
-      </c>
-      <c r="D18" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
WIP to error handling. Stanby due to change BP and relays pining. Special branch : relayChange
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E317C90-A6F7-422D-8068-6E594D52FC11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B89DB9B-B0B2-469B-87E2-A1F5C7A805CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="114">
   <si>
     <t>Nom du test</t>
   </si>
@@ -213,9 +213,6 @@
     <t>LOW</t>
   </si>
   <si>
-    <t>No RTC (in station mode connected and NTP accessible</t>
-  </si>
-  <si>
     <t>No RTC (in station mode connected and no NTP accessible</t>
   </si>
   <si>
@@ -273,9 +270,6 @@
     <t>WiFi Ok mais pas d'internet</t>
   </si>
   <si>
-    <t>Pas de json pour l'interface</t>
-  </si>
-  <si>
     <t>passer à la version light de l'interface</t>
   </si>
   <si>
@@ -331,10 +325,6 @@
   </si>
   <si>
     <t>credential : wrong structure</t>
-  </si>
-  <si>
-    <t>if Station mode connected and NTP server
-No for first release we considere that when a compooennt such RTC is ko all EPS is ko</t>
   </si>
   <si>
     <t>Server could be temporary down</t>
@@ -360,13 +350,56 @@
   </si>
   <si>
     <t>no I2C bus @ powerup</t>
+  </si>
+  <si>
+    <t>config param : no access to file &lt;=&gt; config.json no access</t>
+  </si>
+  <si>
+    <t>config param : wrong structure</t>
+  </si>
+  <si>
+    <t>Pas de CDN (boostrap et jQery) pour l'interface</t>
+  </si>
+  <si>
+    <t>implemented</t>
+  </si>
+  <si>
+    <t>To day class ConfigParam dosen't report such detail</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>blue/black</t>
+  </si>
+  <si>
+    <t>red/black</t>
+  </si>
+  <si>
+    <t>instanciat</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if Station mode connected and NTP server
+</t>
+  </si>
+  <si>
+    <t>No RTC (in station mode connected and NTP accessible)</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Fired by rtcErr  ! For all time arrors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,16 +422,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +433,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -420,10 +451,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -439,13 +469,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
-    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,15 +494,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -612,6 +641,56 @@
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
             <a:t>Peut-être getGravityError()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>What is a fatal error ?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>An error that prevent to use simpleManualMode (push button)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>A component HS =&gt; fatal error (example : rtc component DS3231)</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -946,42 +1025,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1042,18 +1121,18 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3">
         <v>43558</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1062,13 +1141,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3">
         <v>43558</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1082,13 +1161,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="3">
         <v>43558</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1096,19 +1175,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="F5" s="3">
         <v>43558</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1119,19 +1198,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="3">
         <v>43558</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1142,13 +1221,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="3">
         <v>43558</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1159,33 +1238,33 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="3">
         <v>43558</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" s="3">
         <v>43558</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,7 +1275,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1286,25 +1365,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="64.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="41.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
@@ -1313,18 +1395,27 @@
         <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>39</v>
@@ -1333,278 +1424,334 @@
         <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>100</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>101</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="C17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP on the road of error Handling...
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B89DB9B-B0B2-469B-87E2-A1F5C7A805CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4C848-4A56-47B8-B47C-C96EB0D8202C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="122">
   <si>
     <t>Nom du test</t>
   </si>
@@ -168,9 +168,6 @@
     <t>No SPIFFS</t>
   </si>
   <si>
-    <t>Acces to config3.json impossible</t>
-  </si>
-  <si>
     <t>No Wifi station</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>Mode dégradé</t>
   </si>
   <si>
-    <t>Only Very simple mode possible</t>
-  </si>
-  <si>
     <t>HIGH</t>
   </si>
   <si>
@@ -328,10 +322,6 @@
   </si>
   <si>
     <t>Server could be temporary down</t>
-  </si>
-  <si>
-    <t>Manual mode ON/OFF with BP
-To return to normal : correct the pb and restart so no need to do in CBIT</t>
   </si>
   <si>
     <t>no for the same reaseons
@@ -379,9 +369,6 @@
     <t>instanciat</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">if Station mode connected and NTP server
 </t>
   </si>
@@ -393,6 +380,44 @@
   </si>
   <si>
     <t>Fired by rtcErr  ! For all time arrors</t>
+  </si>
+  <si>
+    <t>Red/Bleu</t>
+  </si>
+  <si>
+    <t>Manual mode ON/OFF with BP
+To return to normal : correct the pb and restart so no need to do in CBIT
+No : there is no Cparm so Fatal error</t>
+  </si>
+  <si>
+    <t>Only Very simple mode possible : NO</t>
+  </si>
+  <si>
+    <t>OrangeRed/Black</t>
+  </si>
+  <si>
+    <t>Red/Yellow</t>
+  </si>
+  <si>
+    <t>fsErr</t>
+  </si>
+  <si>
+    <t>i2cErr</t>
+  </si>
+  <si>
+    <t>nanoErr</t>
+  </si>
+  <si>
+    <t>Start in mde AP</t>
+  </si>
+  <si>
+    <t>Same as previous</t>
+  </si>
+  <si>
+    <t>confFileErr</t>
+  </si>
+  <si>
+    <t>rtcErr</t>
   </si>
 </sst>
 </file>
@@ -502,7 +527,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -692,7 +717,45 @@
             </a:rPr>
             <a:t>A component HS =&gt; fatal error (example : rtc component DS3231)</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Possible colors are : </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CRGB::Red, CRGB::OrangeRed, CRGB::Brown; //rose,CRGB::Snow; //blanc bleu, CRGB::Chartreuse, CRGB::RoyalBlue, Yellow</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1025,42 +1088,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1121,18 +1184,18 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3">
         <v>43558</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1141,13 +1204,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3">
         <v>43558</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1161,13 +1224,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3">
         <v>43558</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,19 +1238,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3">
         <v>43558</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1198,19 +1261,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="3">
         <v>43558</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1221,13 +1284,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" s="3">
         <v>43558</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1238,33 +1301,33 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F8" s="3">
         <v>43558</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="3">
         <v>43558</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1275,7 +1338,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1365,16 +1428,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
@@ -1386,358 +1449,385 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>53</v>
+      <c r="C2" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>62</v>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>95</v>
+      <c r="G8" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>62</v>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="E15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,11 +1838,6 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A very important improvement of error handling, not completely finished but well advanced. Soma adds to config4.json
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4C848-4A56-47B8-B47C-C96EB0D8202C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ED395D-A6CD-4147-B026-BD4C5F30832D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
   <si>
     <t>Nom du test</t>
   </si>
@@ -186,12 +186,6 @@
     <t xml:space="preserve">Pas de page index HTML </t>
   </si>
   <si>
-    <t>Perte des fichier css</t>
-  </si>
-  <si>
-    <t>liste exhaustive pour vérifier</t>
-  </si>
-  <si>
     <t>Gravity</t>
   </si>
   <si>
@@ -262,9 +256,6 @@
   </si>
   <si>
     <t>WiFi Ok mais pas d'internet</t>
-  </si>
-  <si>
-    <t>passer à la version light de l'interface</t>
   </si>
   <si>
     <t>First boot tests: normal, SSID connect</t>
@@ -354,13 +345,7 @@
     <t>implemented</t>
   </si>
   <si>
-    <t>To day class ConfigParam dosen't report such detail</t>
-  </si>
-  <si>
     <t>color</t>
-  </si>
-  <si>
-    <t>blue/black</t>
   </si>
   <si>
     <t>red/black</t>
@@ -402,15 +387,9 @@
     <t>fsErr</t>
   </si>
   <si>
-    <t>i2cErr</t>
-  </si>
-  <si>
     <t>nanoErr</t>
   </si>
   <si>
-    <t>Start in mde AP</t>
-  </si>
-  <si>
     <t>Same as previous</t>
   </si>
   <si>
@@ -418,6 +397,60 @@
   </si>
   <si>
     <t>rtcErr</t>
+  </si>
+  <si>
+    <t>To day nanoErr and i2cErr are same.
+There is no mean to test I2C bus alone only through rtc or nano the only 2 components connected to the bus</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>FATAL error if nor AP and station mode not accessibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perte des fichier css, js </t>
+  </si>
+  <si>
+    <t>passer à la version light de l'interface
+En signalant dans la page qu'on a pas d'accès à internet
+Pour le tester faire un ping</t>
+  </si>
+  <si>
+    <t>Not a real error see below</t>
+  </si>
+  <si>
+    <t>liste exhaustive pour vérifier, tout ce qui est dans data
+main.js
+plug.js
+regExpatern.js
+table.js
+index.html
+sidebarr.css
+style.css
+firstboot.html (perhaps)
+config.html
+jquery-3.3.1.min.js (à venir)
+bootstrap.min.css (à venir)
+bootstrap.min.js (à venir)</t>
+  </si>
+  <si>
+    <t>filesErr</t>
+  </si>
+  <si>
+    <t>Start in mode AP</t>
+  </si>
+  <si>
+    <t>To day, class ConfigParam dosen't report such detail</t>
+  </si>
+  <si>
+    <t>plug</t>
+  </si>
+  <si>
+    <t>plugParamErr</t>
+  </si>
+  <si>
+    <t>Red/Snow</t>
   </si>
 </sst>
 </file>
@@ -448,7 +481,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +499,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -480,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -495,6 +534,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -521,13 +563,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -755,6 +797,31 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>CRGB::Red, CRGB::OrangeRed, CRGB::Brown; //rose,CRGB::Snow; //blanc bleu, CRGB::Chartreuse, CRGB::RoyalBlue, Yellow</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Information : main power led could be used to signal non fatal error</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1088,42 +1155,42 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1184,18 +1251,18 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3">
         <v>43558</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1204,13 +1271,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3">
         <v>43558</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1224,13 +1291,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F4" s="3">
         <v>43558</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1238,19 +1305,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3">
         <v>43558</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1261,19 +1328,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F6" s="3">
         <v>43558</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1284,13 +1351,13 @@
         <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3">
         <v>43558</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1301,33 +1368,33 @@
         <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F8" s="3">
         <v>43558</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="3">
         <v>43558</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1338,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,363 +1516,342 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" s="2" t="s">
         <v>109</v>
       </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>90</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>54</v>
+        <v>125</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1813,30 +1859,78 @@
         <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>92</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CBIT of ntp server + necessary files...
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0ED395D-A6CD-4147-B026-BD4C5F30832D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB96AE-8937-4868-A9F0-7DE06A0DD39B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -412,11 +412,6 @@
     <t xml:space="preserve">Perte des fichier css, js </t>
   </si>
   <si>
-    <t>passer à la version light de l'interface
-En signalant dans la page qu'on a pas d'accès à internet
-Pour le tester faire un ping</t>
-  </si>
-  <si>
     <t>Not a real error see below</t>
   </si>
   <si>
@@ -451,6 +446,12 @@
   </si>
   <si>
     <t>Red/Snow</t>
+  </si>
+  <si>
+    <t>passer à la version light de l'interface
+En signalant dans la page qu'on a pas d'accès à internet
+Pour le tester faire un ping
+Passé à FATAL le 19/06/2019 : trop chiant. LE but est arrivé enfin au bout du dev.</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1587,7 @@
         <v>85</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>108</v>
@@ -1606,7 +1607,7 @@
         <v>85</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1653,7 +1654,7 @@
         <v>112</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1767,7 +1768,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>58</v>
@@ -1776,10 +1777,10 @@
         <v>86</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -1817,24 +1818,24 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>49</v>
+      <c r="C15" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1882,7 +1883,7 @@
         <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1899,7 +1900,7 @@
         <v>86</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1916,7 +1917,7 @@
         <v>86</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Internet health check ok
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB96AE-8937-4868-A9F0-7DE06A0DD39B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1BB81C-4AED-4A42-BE14-1FAA5119E864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="135">
   <si>
     <t>Nom du test</t>
   </si>
@@ -452,6 +452,28 @@
 En signalant dans la page qu'on a pas d'accès à internet
 Pour le tester faire un ping
 Passé à FATAL le 19/06/2019 : trop chiant. LE but est arrivé enfin au bout du dev.</t>
+  </si>
+  <si>
+    <t>internet</t>
+  </si>
+  <si>
+    <t>no access in station mode only</t>
+  </si>
+  <si>
+    <t>due to the usage of CDN</t>
+  </si>
+  <si>
+    <t>Orange Red/Royal blue</t>
+  </si>
+  <si>
+    <t>Internet access</t>
+  </si>
+  <si>
+    <t>Connect sytem to pi IOT gateway
+Disconnect internet pi access</t>
+  </si>
+  <si>
+    <t>Fatal error blink royal bue and orange Red</t>
   </si>
 </sst>
 </file>
@@ -520,7 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -539,6 +561,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,103 +1123,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6009E7-5EB8-4E17-B18A-0866A3019060}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1498,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,6 +1897,26 @@
         <v>88</v>
       </c>
     </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
watchdog implementation start. Compiled but not tested and a lot of work to do...
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1BB81C-4AED-4A42-BE14-1FAA5119E864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Comon tests" sheetId="3" r:id="rId1"/>
@@ -479,7 +478,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -606,7 +605,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F9365E-C82A-4A20-B8BD-7E202C3B0026}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26F9365E-C82A-4A20-B8BD-7E202C3B0026}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1115,14 +1114,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6009E7-5EB8-4E17-B18A-0866A3019060}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1242,7 +1241,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A8B8F9-5134-4744-A58F-404FFAC0FBF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1537,11 +1536,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1550,7 @@
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>

</xml_diff>

<commit_message>
ATtiny85 I2C WatchDog integrated + some code cleanup
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E29DBA-221F-4C87-9BE9-4EF12B1EE390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comon tests" sheetId="3" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
   <si>
     <t>Nom du test</t>
   </si>
@@ -474,11 +475,20 @@
   <si>
     <t>Fatal error blink royal bue and orange Red</t>
   </si>
+  <si>
+    <t>watch dog component not accessible</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>errWatchdog</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,7 +607,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -605,7 +615,7 @@
         <xdr:cNvPr id="2" name="ZoneTexte 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{26F9365E-C82A-4A20-B8BD-7E202C3B0026}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F9365E-C82A-4A20-B8BD-7E202C3B0026}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -709,6 +719,12 @@
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
             <a:t>errConfigFile</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>errWatchdog</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1114,14 +1130,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1241,7 +1257,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1536,11 +1552,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1565,7 @@
     <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>
@@ -1809,125 +1825,132 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>124</v>
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>124</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="E13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1935,33 +1958,30 @@
         <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1969,7 +1989,7 @@
         <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>52</v>
@@ -1981,18 +2001,35 @@
         <v>122</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>42</v>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All is working ! apparently. It is time to merge.
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E29DBA-221F-4C87-9BE9-4EF12B1EE390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4149CC7-78C2-4E7A-A3EC-4B5D42AF7323}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1555,8 +1555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
just Execel little correction
</commit_message>
<xml_diff>
--- a/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
+++ b/_1_userDoc/_1-1_tests/testAndErrorHandling.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E29DBA-221F-4C87-9BE9-4EF12B1EE390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4282C524-8DA3-4219-86B0-D34AB40D442D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1565,7 +1565,7 @@
     <col min="2" max="2" width="52.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="41.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="34.5703125" style="1" customWidth="1"/>

</xml_diff>